<commit_message>
prior to import from google sheets
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/config/AgeGroups.xlsx
+++ b/owlcms/src/main/resources/config/AgeGroups.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms4\owlcms\src\main\resources\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E476578B-7CBF-4BA5-8059-77031D1C068D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BAFD139-47B2-4494-8146-5070B3B9DD8F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2850" yWindow="1110" windowWidth="21600" windowHeight="11385" xr2:uid="{01539A8D-3184-427F-BFCD-5BC8845E97D5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="841" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="84">
   <si>
     <t>code</t>
   </si>
@@ -285,6 +285,9 @@
   </si>
   <si>
     <t>https://en.wikipedia.org/wiki/List_of_world_records_in_Olympic_weightlifting#Men</t>
+  </si>
+  <si>
+    <t>M999 is the superheavyweight class for each age group</t>
   </si>
 </sst>
 </file>
@@ -684,8 +687,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72A3C3A3-1F2A-4CC6-B0D9-4ABAF6EBF7C5}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection sqref="A1:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,6 +763,9 @@
       <c r="C5">
         <v>49</v>
       </c>
+      <c r="F5">
+        <v>221</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -777,6 +783,9 @@
       <c r="E6">
         <v>264</v>
       </c>
+      <c r="F6">
+        <v>248</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -794,6 +803,9 @@
       <c r="E7">
         <v>293</v>
       </c>
+      <c r="F7">
+        <v>272</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -811,6 +823,9 @@
       <c r="E8">
         <v>328</v>
       </c>
+      <c r="F8">
+        <v>299</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -828,6 +843,9 @@
       <c r="E9">
         <v>347</v>
       </c>
+      <c r="F9">
+        <v>306</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -845,6 +863,9 @@
       <c r="E10">
         <v>372</v>
       </c>
+      <c r="F10">
+        <v>327</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -862,6 +883,9 @@
       <c r="E11">
         <v>371</v>
       </c>
+      <c r="F11">
+        <v>357</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -879,6 +903,9 @@
       <c r="E12">
         <v>397</v>
       </c>
+      <c r="F12">
+        <v>354</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -896,6 +923,9 @@
       <c r="E13">
         <v>392</v>
       </c>
+      <c r="F13">
+        <v>377</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -930,6 +960,12 @@
       <c r="E15">
         <v>432</v>
       </c>
+      <c r="F15">
+        <v>396</v>
+      </c>
+      <c r="H15" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -942,7 +978,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>28</v>
       </c>
@@ -952,8 +988,11 @@
       <c r="C17">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>29</v>
       </c>
@@ -966,8 +1005,11 @@
       <c r="E18">
         <v>179</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -983,8 +1025,11 @@
       <c r="E19">
         <v>206</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
@@ -1000,8 +1045,11 @@
       <c r="E20">
         <v>211</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>41</v>
       </c>
@@ -1017,8 +1065,11 @@
       <c r="E21">
         <v>228</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1034,8 +1085,11 @@
       <c r="E22">
         <v>240</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
@@ -1051,8 +1105,11 @@
       <c r="E23">
         <v>252</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1068,8 +1125,11 @@
       <c r="E24">
         <v>259</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>45</v>
       </c>
@@ -1085,8 +1145,11 @@
       <c r="E25">
         <v>260</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>47</v>
       </c>
@@ -1103,7 +1166,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>70</v>
       </c>
@@ -1118,6 +1181,9 @@
       </c>
       <c r="E27">
         <v>332</v>
+      </c>
+      <c r="F27">
+        <v>255</v>
       </c>
     </row>
   </sheetData>
@@ -1126,6 +1192,7 @@
     <hyperlink ref="H2" r:id="rId2" location="Men" display="https://en.wikipedia.org/wiki/List_of_world_records_in_Olympic_weightlifting - Men" xr:uid="{00523A9F-3008-463C-9B7D-A4F351E39FDE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1136,8 +1203,8 @@
   </sheetPr>
   <dimension ref="A1:U50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection sqref="A1:U50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3797,6 +3864,7 @@
   <autoFilter ref="G1:G50" xr:uid="{B751848B-6243-4CCE-9281-D58686A89242}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3804,8 +3872,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81D42A18-F9BA-4DF8-9234-51A2A08C5F2E}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection sqref="A1:C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4366,5 +4434,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>